<commit_message>
Update .gitignore to exclude Excel temporary files
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,9 @@
   <si>
     <t>보니토</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트이름</t>
   </si>
 </sst>
 </file>
@@ -423,25 +426,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -458,10 +461,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -478,10 +481,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -498,10 +501,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -513,6 +516,26 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>